<commit_message>
Calibrate RCAPEX diet and 18M DSRA funding
</commit_message>
<xml_diff>
--- a/TP_Quant_Validation.xlsx
+++ b/TP_Quant_Validation.xlsx
@@ -1012,10 +1012,10 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="I7" t="n">
-        <v>18</v>
+        <v>16.8</v>
       </c>
     </row>
     <row r="8">
@@ -1041,10 +1041,10 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I8" t="n">
-        <v>22.1</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="9">
@@ -1070,10 +1070,10 @@
         <v>0</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1.65</v>
       </c>
       <c r="I9" t="n">
-        <v>24.1</v>
+        <v>22.45</v>
       </c>
     </row>
     <row r="10">
@@ -1099,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="I10" t="n">
-        <v>25.3</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="11">
@@ -1128,10 +1128,10 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>1.55</v>
       </c>
       <c r="I11" t="n">
-        <v>22.8</v>
+        <v>21.25</v>
       </c>
     </row>
     <row r="12">
@@ -1157,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="I12" t="n">
-        <v>21</v>
+        <v>17.6</v>
       </c>
     </row>
     <row r="13">
@@ -1186,10 +1186,10 @@
         <v>0</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="I13" t="n">
-        <v>19.7</v>
+        <v>17.45</v>
       </c>
     </row>
     <row r="14">
@@ -1215,10 +1215,10 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I14" t="n">
-        <v>17.4</v>
+        <v>15.4</v>
       </c>
     </row>
     <row r="15">
@@ -1244,10 +1244,10 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I15" t="n">
-        <v>15.2</v>
+        <v>13.7</v>
       </c>
     </row>
     <row r="16">
@@ -1273,10 +1273,10 @@
         <v>0</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="I16" t="n">
-        <v>13</v>
+        <v>11.75</v>
       </c>
     </row>
     <row r="17">
@@ -1285,22 +1285,29 @@
           <t>Totals</t>
         </is>
       </c>
-      <c r="B17">
-        <f>SUM(B2:B16)</f>
-        <v/>
-      </c>
-      <c r="C17">
-        <f>SUM(C2:C16)</f>
-        <v/>
-      </c>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17">
-        <f>SUM(I2:I16)</f>
-        <v/>
+      <c r="B17" t="n">
+        <v>360</v>
+      </c>
+      <c r="C17" t="n">
+        <v>121.7</v>
+      </c>
+      <c r="D17" t="n">
+        <v>7.899999999999999</v>
+      </c>
+      <c r="E17" t="n">
+        <v>5.400000000000001</v>
+      </c>
+      <c r="F17" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>36</v>
+      </c>
+      <c r="I17" t="n">
+        <v>178.5</v>
       </c>
     </row>
   </sheetData>
@@ -1966,7 +1973,7 @@
         <v>5.31</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1129943502824859</v>
+        <v>-0.112994350282</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1990,7 +1997,7 @@
         <v>5.31</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.2259887005649718</v>
+        <v>-0.225988700565</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -2014,7 +2021,7 @@
         <v>5.31</v>
       </c>
       <c r="D4" t="n">
-        <v>0.05649717514124294</v>
+        <v>0.056497175141</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -2038,7 +2045,7 @@
         <v>5.31</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9416195856873824</v>
+        <v>0.941619585687</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -2062,7 +2069,7 @@
         <v>8.551724999999999</v>
       </c>
       <c r="D6" t="n">
-        <v>1.44999985383066</v>
+        <v>1.449999853831</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -2071,7 +2078,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BREACH</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2080,13 +2087,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>18</v>
+        <v>16.8</v>
       </c>
       <c r="C7" t="n">
         <v>12.413794</v>
       </c>
       <c r="D7" t="n">
-        <v>1.449999895277785</v>
+        <v>1.353333235593</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2104,13 +2111,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>22.1</v>
+        <v>20.6</v>
       </c>
       <c r="C8" t="n">
         <v>15.24138</v>
       </c>
       <c r="D8" t="n">
-        <v>1.449999934389143</v>
+        <v>1.35158364925</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2119,7 +2126,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BREACH</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2128,13 +2135,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>24.1</v>
+        <v>22.45</v>
       </c>
       <c r="C9" t="n">
         <v>16.62069</v>
       </c>
       <c r="D9" t="n">
-        <v>1.449999969917013</v>
+        <v>1.350726113055</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -2143,7 +2150,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BREACH</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2152,13 +2159,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>25.3</v>
+        <v>23.6</v>
       </c>
       <c r="C10" t="n">
         <v>17.448276</v>
       </c>
       <c r="D10" t="n">
-        <v>1.44999998853755</v>
+        <v>1.352569159268</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -2167,7 +2174,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>BREACH</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -2176,13 +2183,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>22.8</v>
+        <v>21.25</v>
       </c>
       <c r="C11" t="n">
         <v>15.724137</v>
       </c>
       <c r="D11" t="n">
-        <v>1.450000085855268</v>
+        <v>1.351425518615</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2191,7 +2198,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>BREACH</t>
         </is>
       </c>
     </row>
@@ -2200,13 +2207,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>21</v>
+        <v>17.6</v>
       </c>
       <c r="C12" t="n">
         <v>10.705504</v>
       </c>
       <c r="D12" t="n">
-        <v>1.961607786050988</v>
+        <v>1.6440141445</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2224,14 +2231,11 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>19.7</v>
+        <v>17.45</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
-      <c r="D13" t="n">
-        <v/>
-      </c>
       <c r="E13" t="inlineStr">
         <is>
           <t>post</t>
@@ -2239,7 +2243,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2248,14 +2252,11 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>17.4</v>
+        <v>15.4</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
-      <c r="D14" t="n">
-        <v/>
-      </c>
       <c r="E14" t="inlineStr">
         <is>
           <t>post</t>
@@ -2263,7 +2264,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2272,14 +2273,11 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>15.2</v>
+        <v>13.7</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
-      <c r="D15" t="n">
-        <v/>
-      </c>
       <c r="E15" t="inlineStr">
         <is>
           <t>post</t>
@@ -2287,7 +2285,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2296,14 +2294,11 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>13</v>
+        <v>11.75</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
-      <c r="D16" t="n">
-        <v/>
-      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>post</t>
@@ -2311,7 +2306,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
@@ -2512,11 +2507,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>214.5</v>
-      </c>
-      <c r="C2">
-        <f>CFADS_Calc!I17</f>
-        <v/>
+        <v>196.5</v>
+      </c>
+      <c r="C2" t="n">
+        <v>196.5</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -2534,11 +2528,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1.44999985383066</v>
-      </c>
-      <c r="C3">
-        <f>Ratios!D6</f>
-        <v/>
+        <v>1.449999853831</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.449999853831</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
@@ -2556,11 +2549,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.961607786050988</v>
-      </c>
-      <c r="C4">
-        <f>Ratios!D12</f>
-        <v/>
+        <v>1.6440141445</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1.6440141445</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>

</xml_diff>